<commit_message>
feature update: bokeh chart added to dashboard
</commit_message>
<xml_diff>
--- a/misc/big_table6_fix170_with_trim.xlsx
+++ b/misc/big_table6_fix170_with_trim.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60df6d5feed7ac60/Documents/professional/20210710lifeBuddy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60df6d5feed7ac60/Documents/professional/20210710lifeBuddy/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_A48EDFC8B0A92FFBA6170BE7AB5DF7CF512DCB6B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B01821E6-CB01-423B-B69F-6788C30C2D10}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_A48EDFC8B0A92FFBA6170BE7AB5DF7CF512DCB6B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AF16E95-9623-46C1-890A-4E0F4DBB45CC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21630" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$225</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1230,23 +1241,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E161" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
+      <selection pane="bottomRight" activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="83.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1277,7 +1288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1303,7 +1314,7 @@
         <v>-189.62737001650211</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1329,7 +1340,7 @@
         <v>-15.319679410178781</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1355,7 +1366,7 @@
         <v>-12.588130137881681</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1381,7 +1392,7 @@
         <v>-11.740647000690039</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1409,31 +1420,31 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="B7" t="s">
         <v>235</v>
       </c>
       <c r="C7">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D7">
-        <v>485</v>
+        <v>2349</v>
       </c>
       <c r="E7" s="2">
-        <v>9.9230972876141266</v>
+        <v>56.367650952476048</v>
       </c>
       <c r="F7" s="2">
-        <v>4.3715574749031054</v>
+        <v>44.360098312792537</v>
       </c>
       <c r="G7" s="2">
-        <v>0.34726410521612783</v>
+        <v>-5.2393463200689272E-2</v>
       </c>
       <c r="H7" s="2">
-        <v>-1.141270932171323</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-1.8708621158115251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1459,7 +1470,7 @@
         <v>-21.85078406606582</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1485,7 +1496,7 @@
         <v>-12.25578049320149</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1511,7 +1522,7 @@
         <v>-30.591672729858459</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1539,31 +1550,31 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>227</v>
       </c>
       <c r="B12" t="s">
         <v>235</v>
       </c>
       <c r="C12">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="D12">
-        <v>342</v>
+        <v>2210</v>
       </c>
       <c r="E12" s="2">
-        <v>4.2806989780620777</v>
+        <v>34.09935547955277</v>
       </c>
       <c r="F12" s="2">
-        <v>1.9348043092219409</v>
+        <v>25.097487683304269</v>
       </c>
       <c r="G12" s="2">
-        <v>2.072359862721318E-2</v>
+        <v>0.60528078994653289</v>
       </c>
       <c r="H12" s="2">
-        <v>-0.58796948427583873</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.27772600976664891</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1589,7 +1600,7 @@
         <v>-16.831152572606651</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1617,31 +1628,31 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
         <v>235</v>
       </c>
       <c r="C15">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D15">
-        <v>1094</v>
+        <v>2186</v>
       </c>
       <c r="E15" s="2">
-        <v>23.702082124148099</v>
+        <v>49.7709260032087</v>
       </c>
       <c r="F15" s="2">
-        <v>14.16734132948794</v>
+        <v>38.413480744349577</v>
       </c>
       <c r="G15" s="2">
-        <v>0.72947244098844111</v>
+        <v>0.60373064869819348</v>
       </c>
       <c r="H15" s="2">
-        <v>-0.16566023655277881</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-1.717122341320931E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1667,7 +1678,7 @@
         <v>-13.1206176798266</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1694,32 +1705,32 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="A18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C18">
-        <v>156</v>
-      </c>
-      <c r="D18">
-        <v>143</v>
-      </c>
-      <c r="E18" s="2">
-        <v>9.2480746628223827</v>
-      </c>
-      <c r="F18" s="2">
-        <v>3.2584483755467062</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0.2240466170549216</v>
-      </c>
-      <c r="H18" s="2">
-        <v>-4.5154638744299476</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="3">
+        <v>170</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2161</v>
+      </c>
+      <c r="E18" s="4">
+        <v>40.639151915039157</v>
+      </c>
+      <c r="F18" s="4">
+        <v>30.997978807673199</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.7992281593234406</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.42334686427122092</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1745,7 +1756,7 @@
         <v>-16.056345835052781</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1771,7 +1782,7 @@
         <v>-17.247649722067351</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1797,7 +1808,7 @@
         <v>-6.3877554464932356</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1823,7 +1834,7 @@
         <v>-13.46923674491881</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1849,7 +1860,7 @@
         <v>-4.5938624802457513</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1875,7 +1886,7 @@
         <v>-14.782631519903861</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1901,7 +1912,7 @@
         <v>-12.616765814546071</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1927,7 +1938,7 @@
         <v>-4.716860240178347</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1953,7 +1964,7 @@
         <v>-13.186391413919679</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1979,7 +1990,7 @@
         <v>-7.802199170110347</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -2007,31 +2018,31 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>198</v>
       </c>
       <c r="B30" t="s">
         <v>235</v>
       </c>
       <c r="C30">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="D30">
-        <v>154</v>
+        <v>2144</v>
       </c>
       <c r="E30" s="2">
-        <v>7.4510885553505473</v>
+        <v>51.077433540844339</v>
       </c>
       <c r="F30" s="2">
-        <v>2.492613749837882</v>
+        <v>40.992026741200952</v>
       </c>
       <c r="G30" s="2">
-        <v>-0.22931039018344901</v>
+        <v>0.7654020870411935</v>
       </c>
       <c r="H30" s="2">
-        <v>-7.1801972159013054</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.56724965371820535</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -2057,7 +2068,7 @@
         <v>-28.477133979176781</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -2083,7 +2094,7 @@
         <v>-19.146968359420701</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -2109,7 +2120,7 @@
         <v>-1.262127794831015</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -2135,7 +2146,7 @@
         <v>-70.53695523200264</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2161,7 +2172,7 @@
         <v>-11.97611113034524</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -2189,31 +2200,31 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
         <v>235</v>
       </c>
       <c r="C37">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D37">
-        <v>1314</v>
+        <v>2032</v>
       </c>
       <c r="E37" s="2">
-        <v>36.447561164580613</v>
+        <v>53.555175588071833</v>
       </c>
       <c r="F37" s="2">
-        <v>27.912296939202641</v>
+        <v>43.69484701547352</v>
       </c>
       <c r="G37" s="2">
-        <v>-1.041929065082055</v>
+        <v>0.6777009151181812</v>
       </c>
       <c r="H37" s="2">
-        <v>-1.840640625698007</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.33052273150410999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -2239,7 +2250,7 @@
         <v>-64.071447867082824</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2265,7 +2276,7 @@
         <v>-20.281722723652631</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -2291,7 +2302,7 @@
         <v>-9.3953841631413919</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -2317,7 +2328,7 @@
         <v>-13.147122540199531</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2345,31 +2356,31 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="B43" t="s">
         <v>235</v>
       </c>
       <c r="C43">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="D43">
-        <v>153</v>
+        <v>1937</v>
       </c>
       <c r="E43" s="2">
-        <v>6.8862617191842768</v>
+        <v>23.284460426358979</v>
       </c>
       <c r="F43" s="2">
-        <v>2.7375989327663461</v>
+        <v>14.69072098814779</v>
       </c>
       <c r="G43" s="2">
-        <v>0.15723303348140469</v>
+        <v>0.74589065992419568</v>
       </c>
       <c r="H43" s="2">
-        <v>-0.23697828441389679</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.18791108356816791</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2395,7 +2406,7 @@
         <v>-10.393876203489</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -2423,31 +2434,31 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>197</v>
       </c>
       <c r="B46" t="s">
         <v>235</v>
       </c>
       <c r="C46">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D46">
-        <v>1197</v>
+        <v>1861</v>
       </c>
       <c r="E46" s="2">
-        <v>26.236377325775411</v>
+        <v>51.237006837878148</v>
       </c>
       <c r="F46" s="2">
-        <v>16.684753953261389</v>
+        <v>42.150823841330137</v>
       </c>
       <c r="G46" s="2">
-        <v>0.78041108809509196</v>
+        <v>-0.20743265675368711</v>
       </c>
       <c r="H46" s="2">
-        <v>0.23682507576790271</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-1.2061158637620739</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -2473,7 +2484,7 @@
         <v>-6.8380146617077484E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -2499,7 +2510,7 @@
         <v>-2.3545920167007379</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -2526,32 +2537,32 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="3" t="s">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" t="s">
         <v>235</v>
       </c>
-      <c r="C50" s="3">
-        <v>170</v>
-      </c>
-      <c r="D50" s="3">
-        <v>2161</v>
-      </c>
-      <c r="E50" s="4">
-        <v>40.639151915039157</v>
-      </c>
-      <c r="F50" s="4">
-        <v>30.997978807673199</v>
-      </c>
-      <c r="G50" s="4">
-        <v>0.7992281593234406</v>
-      </c>
-      <c r="H50" s="4">
-        <v>0.42334686427122092</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>169</v>
+      </c>
+      <c r="D50">
+        <v>1617</v>
+      </c>
+      <c r="E50" s="2">
+        <v>35.249572346319887</v>
+      </c>
+      <c r="F50" s="2">
+        <v>23.787069956749029</v>
+      </c>
+      <c r="G50" s="2">
+        <v>-0.68809117829536826</v>
+      </c>
+      <c r="H50" s="2">
+        <v>-1.284242527812689</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -2579,31 +2590,31 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>225</v>
       </c>
       <c r="B52" t="s">
         <v>235</v>
       </c>
       <c r="C52">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D52">
-        <v>1617</v>
+        <v>1527</v>
       </c>
       <c r="E52" s="2">
-        <v>35.249572346319887</v>
+        <v>51.81160325854551</v>
       </c>
       <c r="F52" s="2">
-        <v>23.787069956749029</v>
+        <v>47.611500018495519</v>
       </c>
       <c r="G52" s="2">
-        <v>-0.68809117829536826</v>
+        <v>-2.3406745201743449</v>
       </c>
       <c r="H52" s="2">
-        <v>-1.284242527812689</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-2.4564784967956141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2629,7 +2640,7 @@
         <v>-53.308431572094683</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2655,7 +2666,7 @@
         <v>-116.0698958709913</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -2681,7 +2692,7 @@
         <v>-14.23305995177277</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2709,31 +2720,31 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="B57" t="s">
         <v>235</v>
       </c>
       <c r="C57">
-        <v>145</v>
+        <v>174</v>
       </c>
       <c r="D57">
-        <v>631</v>
+        <v>1508</v>
       </c>
       <c r="E57" s="2">
-        <v>72.706065834208061</v>
+        <v>32.790227108914472</v>
       </c>
       <c r="F57" s="2">
-        <v>62.08363502336428</v>
+        <v>22.027990079217901</v>
       </c>
       <c r="G57" s="2">
-        <v>-2.52267372068617</v>
+        <v>-0.5275977354059338</v>
       </c>
       <c r="H57" s="2">
-        <v>-6.3628819004968991</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-1.0710783711782339</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2759,7 +2770,7 @@
         <v>-4.8323959042028157</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2785,7 +2796,7 @@
         <v>-2.5404008350929721</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2813,7 +2824,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="B61" t="s">
         <v>235</v>
@@ -2822,22 +2833,22 @@
         <v>170</v>
       </c>
       <c r="D61">
-        <v>627</v>
+        <v>1365</v>
       </c>
       <c r="E61" s="2">
-        <v>17.81276788342392</v>
+        <v>36.467101619170073</v>
       </c>
       <c r="F61" s="2">
-        <v>10.903242520630389</v>
+        <v>24.811016855272399</v>
       </c>
       <c r="G61" s="2">
-        <v>0.63844839407361575</v>
+        <v>-0.24346258400294449</v>
       </c>
       <c r="H61" s="2">
-        <v>0.44633543691755317</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-0.91776507026003151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -2865,31 +2876,31 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B63" t="s">
         <v>235</v>
       </c>
       <c r="C63">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="D63">
-        <v>555</v>
+        <v>1314</v>
       </c>
       <c r="E63" s="2">
-        <v>6.1281971754748579</v>
+        <v>36.447561164580613</v>
       </c>
       <c r="F63" s="2">
-        <v>2.282082042842533</v>
+        <v>27.912296939202641</v>
       </c>
       <c r="G63" s="2">
-        <v>0.49351626872891341</v>
+        <v>-1.041929065082055</v>
       </c>
       <c r="H63" s="2">
-        <v>-9.5907613143140669E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-1.840640625698007</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -2917,31 +2928,31 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>156</v>
       </c>
       <c r="B65" t="s">
         <v>235</v>
       </c>
       <c r="C65">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D65">
-        <v>2032</v>
+        <v>1253</v>
       </c>
       <c r="E65" s="2">
-        <v>53.555175588071833</v>
+        <v>49.779274108954162</v>
       </c>
       <c r="F65" s="2">
-        <v>43.69484701547352</v>
+        <v>39.906900062164027</v>
       </c>
       <c r="G65" s="2">
-        <v>0.6777009151181812</v>
+        <v>0.23416164895738459</v>
       </c>
       <c r="H65" s="2">
-        <v>0.33052273150410999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-0.96788056000676259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -2967,7 +2978,7 @@
         <v>0.24443308528026031</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -2995,31 +3006,31 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="B68" t="s">
         <v>235</v>
       </c>
       <c r="C68">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D68">
-        <v>2186</v>
+        <v>1210</v>
       </c>
       <c r="E68" s="2">
-        <v>49.7709260032087</v>
+        <v>43.648880939463382</v>
       </c>
       <c r="F68" s="2">
-        <v>38.413480744349577</v>
+        <v>34.755333455994311</v>
       </c>
       <c r="G68" s="2">
-        <v>0.60373064869819348</v>
+        <v>0.2260128447834524</v>
       </c>
       <c r="H68" s="2">
-        <v>-1.717122341320931E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-0.18487144114729559</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -3045,7 +3056,7 @@
         <v>-19.567258610129741</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -3071,7 +3082,7 @@
         <v>0.35488965235690889</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -3097,7 +3108,7 @@
         <v>-0.53980755202000563</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -3125,31 +3136,31 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="B73" t="s">
         <v>235</v>
       </c>
       <c r="C73">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D73">
-        <v>1010</v>
+        <v>1197</v>
       </c>
       <c r="E73" s="2">
-        <v>25.273337759527919</v>
+        <v>26.236377325775411</v>
       </c>
       <c r="F73" s="2">
-        <v>16.003017959298141</v>
+        <v>16.684753953261389</v>
       </c>
       <c r="G73" s="2">
-        <v>0.78156790607676696</v>
+        <v>0.78041108809509196</v>
       </c>
       <c r="H73" s="2">
-        <v>0.19844893511416509</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.23682507576790271</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -3175,7 +3186,7 @@
         <v>-3.732078894318926</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -3201,7 +3212,7 @@
         <v>-3.742438949581063</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -3227,7 +3238,7 @@
         <v>-17.595123486257229</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -3253,7 +3264,7 @@
         <v>-6.8798767509133132</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -3279,7 +3290,7 @@
         <v>-13.65428988213128</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -3305,7 +3316,7 @@
         <v>-3.6984729198552557E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -3331,7 +3342,7 @@
         <v>-8.9658150505894678</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -3357,7 +3368,7 @@
         <v>-8.6383091019801892</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -3383,7 +3394,7 @@
         <v>-9.1492095176828894</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -3409,7 +3420,7 @@
         <v>-57.831974035391859</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -3435,7 +3446,7 @@
         <v>-24.55918128658454</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -3461,7 +3472,7 @@
         <v>-9.8730567875085562</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -3487,7 +3498,7 @@
         <v>-8.7309304337177984</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -3513,7 +3524,7 @@
         <v>-0.15792667388067769</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -3539,7 +3550,7 @@
         <v>0.57843706048152743</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -3565,7 +3576,7 @@
         <v>-0.37966902408159758</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -3591,7 +3602,7 @@
         <v>-29.7327713532964</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -3617,7 +3628,7 @@
         <v>-5.4529859258461579</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -3643,7 +3654,7 @@
         <v>-11.181762871717609</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -3669,7 +3680,7 @@
         <v>-13.993673631674881</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -3695,7 +3706,7 @@
         <v>-16.749376081323948</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -3721,7 +3732,7 @@
         <v>-16.976989081991121</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -3747,7 +3758,7 @@
         <v>-155.7822759749202</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -3773,7 +3784,7 @@
         <v>-2.086001310032271</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -3799,7 +3810,7 @@
         <v>-12.09252614524069</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -3825,7 +3836,7 @@
         <v>-3.889748695011344</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -3853,31 +3864,31 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="B101" t="s">
         <v>235</v>
       </c>
       <c r="C101">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="D101">
-        <v>1508</v>
+        <v>1175</v>
       </c>
       <c r="E101" s="2">
-        <v>32.790227108914472</v>
+        <v>39.97566582969273</v>
       </c>
       <c r="F101" s="2">
-        <v>22.027990079217901</v>
+        <v>28.941827434537348</v>
       </c>
       <c r="G101" s="2">
-        <v>-0.5275977354059338</v>
+        <v>-0.63953932009518333</v>
       </c>
       <c r="H101" s="2">
-        <v>-1.0710783711782339</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-3.0399006229029282</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>108</v>
       </c>
@@ -3903,7 +3914,7 @@
         <v>0.2372604988678568</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>109</v>
       </c>
@@ -3931,31 +3942,31 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>110</v>
+        <v>202</v>
       </c>
       <c r="B104" t="s">
         <v>235</v>
       </c>
       <c r="C104">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D104">
-        <v>1365</v>
+        <v>1151</v>
       </c>
       <c r="E104" s="2">
-        <v>36.467101619170073</v>
+        <v>24.327181009889038</v>
       </c>
       <c r="F104" s="2">
-        <v>24.811016855272399</v>
+        <v>15.65089264781715</v>
       </c>
       <c r="G104" s="2">
-        <v>-0.24346258400294449</v>
+        <v>0.77670560058028415</v>
       </c>
       <c r="H104" s="2">
-        <v>-0.91776507026003151</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.1667301787084069</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -3983,31 +3994,31 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>112</v>
+        <v>199</v>
       </c>
       <c r="B106" t="s">
         <v>235</v>
       </c>
       <c r="C106">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D106">
-        <v>161</v>
+        <v>1141</v>
       </c>
       <c r="E106" s="2">
-        <v>4.5657843463384751</v>
+        <v>33.278026717264829</v>
       </c>
       <c r="F106" s="2">
-        <v>1.190512081949846</v>
+        <v>22.63325993496046</v>
       </c>
       <c r="G106" s="2">
-        <v>0.17920735823326589</v>
+        <v>0.90630011281332379</v>
       </c>
       <c r="H106" s="2">
-        <v>-1.921188741160909</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.65292235159799594</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -4033,7 +4044,7 @@
         <v>-21.469288546721259</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -4059,7 +4070,7 @@
         <v>-18.750943402800392</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -4085,7 +4096,7 @@
         <v>-4.3865942132063713</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -4113,31 +4124,31 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="B111" t="s">
         <v>235</v>
       </c>
       <c r="C111">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="D111">
-        <v>720</v>
+        <v>1128</v>
       </c>
       <c r="E111" s="2">
-        <v>37.511614734920997</v>
+        <v>28.382699055919041</v>
       </c>
       <c r="F111" s="2">
-        <v>27.298656397569889</v>
+        <v>20.330514441811552</v>
       </c>
       <c r="G111" s="2">
-        <v>0.7500718811964624</v>
+        <v>0.79433150667680597</v>
       </c>
       <c r="H111" s="2">
-        <v>0.27747952611528021</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.67620009786334812</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -4163,7 +4174,7 @@
         <v>-5.3106668298650783</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -4189,7 +4200,7 @@
         <v>-232.29573766357561</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -4215,7 +4226,7 @@
         <v>-12.49740745955906</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>121</v>
       </c>
@@ -4241,7 +4252,7 @@
         <v>-22.30059681918847</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>122</v>
       </c>
@@ -4267,7 +4278,7 @@
         <v>-36.794342528920048</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -4293,7 +4304,7 @@
         <v>-13.14622193251266</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>124</v>
       </c>
@@ -4319,7 +4330,7 @@
         <v>-10.858808780874201</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -4345,7 +4356,7 @@
         <v>-20.580249288306788</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -4373,31 +4384,31 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>127</v>
+        <v>21</v>
       </c>
       <c r="B121" t="s">
         <v>235</v>
       </c>
       <c r="C121">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D121">
-        <v>177</v>
+        <v>1094</v>
       </c>
       <c r="E121" s="2">
-        <v>6.8386643742301301</v>
+        <v>23.702082124148099</v>
       </c>
       <c r="F121" s="2">
-        <v>2.137101115036105</v>
+        <v>14.16734132948794</v>
       </c>
       <c r="G121" s="2">
-        <v>0.37016696058476473</v>
+        <v>0.72947244098844111</v>
       </c>
       <c r="H121" s="2">
-        <v>-1.5905015295928231</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-0.16566023655277881</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>128</v>
       </c>
@@ -4425,31 +4436,31 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="B123" t="s">
         <v>235</v>
       </c>
       <c r="C123">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="D123">
-        <v>156</v>
+        <v>1010</v>
       </c>
       <c r="E123" s="2">
-        <v>10.24904502767893</v>
+        <v>25.273337759527919</v>
       </c>
       <c r="F123" s="2">
-        <v>3.9043811765291072</v>
+        <v>16.003017959298141</v>
       </c>
       <c r="G123" s="2">
-        <v>-0.18614511927025121</v>
+        <v>0.78156790607676696</v>
       </c>
       <c r="H123" s="2">
-        <v>-8.5752698737579003</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.19844893511416509</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>130</v>
       </c>
@@ -4475,7 +4486,7 @@
         <v>-12.38585858411351</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>131</v>
       </c>
@@ -4501,7 +4512,7 @@
         <v>-79.668137016783064</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>132</v>
       </c>
@@ -4527,7 +4538,7 @@
         <v>-4.7971212338219207</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>133</v>
       </c>
@@ -4553,7 +4564,7 @@
         <v>-23.976733890019549</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>134</v>
       </c>
@@ -4579,7 +4590,7 @@
         <v>-3.5629254602937919</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>135</v>
       </c>
@@ -4607,31 +4618,31 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>136</v>
+        <v>222</v>
       </c>
       <c r="B130" t="s">
         <v>235</v>
       </c>
       <c r="C130">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="D130">
-        <v>453</v>
+        <v>991</v>
       </c>
       <c r="E130" s="2">
-        <v>22.240123884150918</v>
+        <v>0.51200329043375148</v>
       </c>
       <c r="F130" s="2">
-        <v>13.386517427513921</v>
+        <v>0.37918877089989661</v>
       </c>
       <c r="G130" s="2">
-        <v>0.64731364834751415</v>
+        <v>-0.50871948802159372</v>
       </c>
       <c r="H130" s="2">
-        <v>-0.40320654350607787</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-0.50341315198099523</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -4657,7 +4668,7 @@
         <v>-9.9741162412897921</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>138</v>
       </c>
@@ -4685,31 +4696,31 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="B133" t="s">
         <v>235</v>
       </c>
       <c r="C133">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D133">
-        <v>1937</v>
+        <v>907</v>
       </c>
       <c r="E133" s="2">
-        <v>23.284460426358979</v>
+        <v>25.267661754656199</v>
       </c>
       <c r="F133" s="2">
-        <v>14.69072098814779</v>
+        <v>15.98593906434791</v>
       </c>
       <c r="G133" s="2">
-        <v>0.74589065992419568</v>
+        <v>0.79194939920962204</v>
       </c>
       <c r="H133" s="2">
-        <v>0.18791108356816791</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.4094920091078571</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>140</v>
       </c>
@@ -4735,7 +4746,7 @@
         <v>-32.008075822045932</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>141</v>
       </c>
@@ -4761,7 +4772,7 @@
         <v>-37.207605028888743</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>142</v>
       </c>
@@ -4787,7 +4798,7 @@
         <v>-1.429604863611454</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>143</v>
       </c>
@@ -4813,7 +4824,7 @@
         <v>-0.45135433098756289</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>144</v>
       </c>
@@ -4839,7 +4850,7 @@
         <v>-3.867347091801046</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>145</v>
       </c>
@@ -4867,31 +4878,31 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>146</v>
+        <v>207</v>
       </c>
       <c r="B140" t="s">
         <v>235</v>
       </c>
       <c r="C140">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D140">
-        <v>854</v>
+        <v>888</v>
       </c>
       <c r="E140" s="2">
-        <v>19.015059369243041</v>
+        <v>14.25468076265506</v>
       </c>
       <c r="F140" s="2">
-        <v>11.85178608612417</v>
+        <v>9.8052769505345783</v>
       </c>
       <c r="G140" s="2">
-        <v>0.74785970118485467</v>
+        <v>-0.44422008972081861</v>
       </c>
       <c r="H140" s="2">
-        <v>0.43295815877124172</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-1.626183012561373</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>147</v>
       </c>
@@ -4917,7 +4928,7 @@
         <v>-18.46403096282739</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>148</v>
       </c>
@@ -4943,7 +4954,7 @@
         <v>-25.43060017965902</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>149</v>
       </c>
@@ -4969,7 +4980,7 @@
         <v>-18.131045578759249</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>150</v>
       </c>
@@ -4997,83 +5008,83 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B145" t="s">
         <v>235</v>
       </c>
       <c r="C145">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D145">
-        <v>259</v>
+        <v>854</v>
       </c>
       <c r="E145" s="2">
-        <v>3.8681475036345692</v>
+        <v>19.015059369243041</v>
       </c>
       <c r="F145" s="2">
-        <v>1.1947031571622371</v>
+        <v>11.85178608612417</v>
       </c>
       <c r="G145" s="2">
-        <v>-0.122229756286278</v>
+        <v>0.74785970118485467</v>
       </c>
       <c r="H145" s="2">
-        <v>-2.68207200655627</v>
+        <v>0.43295815877124172</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="B146" t="s">
         <v>235</v>
       </c>
       <c r="C146">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D146">
-        <v>1210</v>
+        <v>720</v>
       </c>
       <c r="E146" s="2">
-        <v>43.648880939463382</v>
+        <v>37.511614734920997</v>
       </c>
       <c r="F146" s="2">
-        <v>34.755333455994311</v>
+        <v>27.298656397569889</v>
       </c>
       <c r="G146" s="2">
-        <v>0.2260128447834524</v>
+        <v>0.7500718811964624</v>
       </c>
       <c r="H146" s="2">
-        <v>-0.18487144114729559</v>
+        <v>0.27747952611528021</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>153</v>
+        <v>210</v>
       </c>
       <c r="B147" t="s">
         <v>235</v>
       </c>
       <c r="C147">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D147">
-        <v>907</v>
+        <v>697</v>
       </c>
       <c r="E147" s="2">
-        <v>25.267661754656199</v>
+        <v>26.414769697463729</v>
       </c>
       <c r="F147" s="2">
-        <v>15.98593906434791</v>
+        <v>17.590745763539172</v>
       </c>
       <c r="G147" s="2">
-        <v>0.79194939920962204</v>
+        <v>0.85967870253516132</v>
       </c>
       <c r="H147" s="2">
-        <v>0.4094920091078571</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.52585421434142776</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>154</v>
       </c>
@@ -5099,7 +5110,7 @@
         <v>-6.8903497650441228</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>155</v>
       </c>
@@ -5127,31 +5138,31 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>156</v>
+        <v>63</v>
       </c>
       <c r="B150" t="s">
         <v>235</v>
       </c>
       <c r="C150">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="D150">
-        <v>1253</v>
+        <v>631</v>
       </c>
       <c r="E150" s="2">
-        <v>49.779274108954162</v>
+        <v>72.706065834208061</v>
       </c>
       <c r="F150" s="2">
-        <v>39.906900062164027</v>
+        <v>62.08363502336428</v>
       </c>
       <c r="G150" s="2">
-        <v>0.23416164895738459</v>
+        <v>-2.52267372068617</v>
       </c>
       <c r="H150" s="2">
-        <v>-0.96788056000676259</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-6.3628819004968991</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>157</v>
       </c>
@@ -5177,7 +5188,7 @@
         <v>-0.26908230769137059</v>
       </c>
     </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>158</v>
       </c>
@@ -5203,7 +5214,7 @@
         <v>-14.33115496264678</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>159</v>
       </c>
@@ -5229,7 +5240,7 @@
         <v>-27.23162015640867</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>160</v>
       </c>
@@ -5255,7 +5266,7 @@
         <v>-43.587344219876577</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>161</v>
       </c>
@@ -5281,7 +5292,7 @@
         <v>-33.415141017525563</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>162</v>
       </c>
@@ -5307,7 +5318,7 @@
         <v>-6.559590841917271</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>163</v>
       </c>
@@ -5333,7 +5344,7 @@
         <v>-64.294991646615074</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>164</v>
       </c>
@@ -5359,7 +5370,7 @@
         <v>-4.7454216678068351</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>165</v>
       </c>
@@ -5385,7 +5396,7 @@
         <v>-8.1102279125020704</v>
       </c>
     </row>
-    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>166</v>
       </c>
@@ -5411,7 +5422,7 @@
         <v>-49.763185553361531</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>167</v>
       </c>
@@ -5437,7 +5448,7 @@
         <v>-11.739034430928781</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>168</v>
       </c>
@@ -5463,7 +5474,7 @@
         <v>-12.16368734803328</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>169</v>
       </c>
@@ -5489,7 +5500,7 @@
         <v>-8.9187901152013414</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>170</v>
       </c>
@@ -5515,7 +5526,7 @@
         <v>-11.50057145362074</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>171</v>
       </c>
@@ -5541,7 +5552,7 @@
         <v>-6.5806158775256218</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>172</v>
       </c>
@@ -5569,31 +5580,31 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>173</v>
+        <v>67</v>
       </c>
       <c r="B167" t="s">
         <v>235</v>
       </c>
       <c r="C167">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D167">
-        <v>1128</v>
+        <v>627</v>
       </c>
       <c r="E167" s="2">
-        <v>28.382699055919041</v>
+        <v>17.81276788342392</v>
       </c>
       <c r="F167" s="2">
-        <v>20.330514441811552</v>
+        <v>10.903242520630389</v>
       </c>
       <c r="G167" s="2">
-        <v>0.79433150667680597</v>
+        <v>0.63844839407361575</v>
       </c>
       <c r="H167" s="2">
-        <v>0.67620009786334812</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.44633543691755317</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>174</v>
       </c>
@@ -5619,7 +5630,7 @@
         <v>-15.53158042078628</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>175</v>
       </c>
@@ -5645,7 +5656,7 @@
         <v>-14.57689897261224</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>176</v>
       </c>
@@ -5671,7 +5682,7 @@
         <v>-24.821799528696729</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>177</v>
       </c>
@@ -5697,7 +5708,7 @@
         <v>5.6153846684547933E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>178</v>
       </c>
@@ -5723,7 +5734,7 @@
         <v>-5.9825986941518732</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>179</v>
       </c>
@@ -5749,7 +5760,7 @@
         <v>-1.9291510662372959</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>180</v>
       </c>
@@ -5775,7 +5786,7 @@
         <v>-8.2136920585684088</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>181</v>
       </c>
@@ -5801,7 +5812,7 @@
         <v>-137.08403254841409</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>182</v>
       </c>
@@ -5827,7 +5838,7 @@
         <v>-25.452382942922689</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>183</v>
       </c>
@@ -5853,7 +5864,7 @@
         <v>-10.12441166065644</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>184</v>
       </c>
@@ -5879,7 +5890,7 @@
         <v>-19.35776178137964</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>185</v>
       </c>
@@ -5905,7 +5916,7 @@
         <v>-9.2316962062470775</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>186</v>
       </c>
@@ -5931,7 +5942,7 @@
         <v>-17.444953719239781</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>187</v>
       </c>
@@ -5957,7 +5968,7 @@
         <v>-13.94837972275948</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>188</v>
       </c>
@@ -5983,7 +5994,7 @@
         <v>-34.185647399385999</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>189</v>
       </c>
@@ -6009,7 +6020,7 @@
         <v>-19.143827619821259</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>190</v>
       </c>
@@ -6037,31 +6048,31 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>191</v>
+        <v>69</v>
       </c>
       <c r="B185" t="s">
         <v>235</v>
       </c>
       <c r="C185">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="D185">
-        <v>507</v>
+        <v>555</v>
       </c>
       <c r="E185" s="2">
-        <v>18.719184590549009</v>
+        <v>6.1281971754748579</v>
       </c>
       <c r="F185" s="2">
-        <v>9.6413252053779068</v>
+        <v>2.282082042842533</v>
       </c>
       <c r="G185" s="2">
-        <v>0.81752431749840271</v>
+        <v>0.49351626872891341</v>
       </c>
       <c r="H185" s="2">
-        <v>-4.8775854751965893E-2</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-9.5907613143140669E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>192</v>
       </c>
@@ -6087,7 +6098,7 @@
         <v>-0.15350827073873671</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>193</v>
       </c>
@@ -6113,7 +6124,7 @@
         <v>-22.35069724829178</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>194</v>
       </c>
@@ -6139,7 +6150,7 @@
         <v>-30.363771465105948</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>195</v>
       </c>
@@ -6167,135 +6178,135 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B190" t="s">
         <v>235</v>
       </c>
       <c r="C190">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D190">
-        <v>2349</v>
+        <v>507</v>
       </c>
       <c r="E190" s="2">
-        <v>56.367650952476048</v>
+        <v>18.719184590549009</v>
       </c>
       <c r="F190" s="2">
-        <v>44.360098312792537</v>
+        <v>9.6413252053779068</v>
       </c>
       <c r="G190" s="2">
-        <v>-5.2393463200689272E-2</v>
+        <v>0.81752431749840271</v>
       </c>
       <c r="H190" s="2">
-        <v>-1.8708621158115251</v>
+        <v>-4.8775854751965893E-2</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>197</v>
+        <v>13</v>
       </c>
       <c r="B191" t="s">
         <v>235</v>
       </c>
       <c r="C191">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D191">
-        <v>1861</v>
+        <v>485</v>
       </c>
       <c r="E191" s="2">
-        <v>51.237006837878148</v>
+        <v>9.9230972876141266</v>
       </c>
       <c r="F191" s="2">
-        <v>42.150823841330137</v>
+        <v>4.3715574749031054</v>
       </c>
       <c r="G191" s="2">
-        <v>-0.20743265675368711</v>
+        <v>0.34726410521612783</v>
       </c>
       <c r="H191" s="2">
-        <v>-1.2061158637620739</v>
+        <v>-1.141270932171323</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>198</v>
+        <v>136</v>
       </c>
       <c r="B192" t="s">
         <v>235</v>
       </c>
       <c r="C192">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="D192">
-        <v>2144</v>
+        <v>453</v>
       </c>
       <c r="E192" s="2">
-        <v>51.077433540844339</v>
+        <v>22.240123884150918</v>
       </c>
       <c r="F192" s="2">
-        <v>40.992026741200952</v>
+        <v>13.386517427513921</v>
       </c>
       <c r="G192" s="2">
-        <v>0.7654020870411935</v>
+        <v>0.64731364834751415</v>
       </c>
       <c r="H192" s="2">
-        <v>0.56724965371820535</v>
+        <v>-0.40320654350607787</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>199</v>
+        <v>18</v>
       </c>
       <c r="B193" t="s">
         <v>235</v>
       </c>
       <c r="C193">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D193">
-        <v>1141</v>
+        <v>342</v>
       </c>
       <c r="E193" s="2">
-        <v>33.278026717264829</v>
+        <v>4.2806989780620777</v>
       </c>
       <c r="F193" s="2">
-        <v>22.63325993496046</v>
+        <v>1.9348043092219409</v>
       </c>
       <c r="G193" s="2">
-        <v>0.90630011281332379</v>
+        <v>2.072359862721318E-2</v>
       </c>
       <c r="H193" s="2">
-        <v>0.65292235159799594</v>
+        <v>-0.58796948427583873</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>200</v>
+        <v>151</v>
       </c>
       <c r="B194" t="s">
         <v>235</v>
       </c>
       <c r="C194">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="D194">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E194" s="2">
-        <v>39.130578556466993</v>
+        <v>3.8681475036345692</v>
       </c>
       <c r="F194" s="2">
-        <v>25.983992300053821</v>
+        <v>1.1947031571622371</v>
       </c>
       <c r="G194" s="2">
-        <v>0.7678545909585377</v>
+        <v>-0.122229756286278</v>
       </c>
       <c r="H194" s="2">
-        <v>0.59617674993638714</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-2.68207200655627</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>201</v>
       </c>
@@ -6323,31 +6334,31 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B196" t="s">
         <v>235</v>
       </c>
       <c r="C196">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="D196">
-        <v>1151</v>
+        <v>255</v>
       </c>
       <c r="E196" s="2">
-        <v>24.327181009889038</v>
+        <v>39.130578556466993</v>
       </c>
       <c r="F196" s="2">
-        <v>15.65089264781715</v>
+        <v>25.983992300053821</v>
       </c>
       <c r="G196" s="2">
-        <v>0.77670560058028415</v>
+        <v>0.7678545909585377</v>
       </c>
       <c r="H196" s="2">
-        <v>0.1667301787084069</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.59617674993638714</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>203</v>
       </c>
@@ -6373,7 +6384,7 @@
         <v>-12.185413659484521</v>
       </c>
     </row>
-    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>204</v>
       </c>
@@ -6399,7 +6410,7 @@
         <v>-5.0012176929710623</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>205</v>
       </c>
@@ -6425,7 +6436,7 @@
         <v>-15.697573560843001</v>
       </c>
     </row>
-    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>206</v>
       </c>
@@ -6453,31 +6464,31 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>207</v>
+        <v>127</v>
       </c>
       <c r="B201" t="s">
         <v>235</v>
       </c>
       <c r="C201">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D201">
-        <v>888</v>
+        <v>177</v>
       </c>
       <c r="E201" s="2">
-        <v>14.25468076265506</v>
+        <v>6.8386643742301301</v>
       </c>
       <c r="F201" s="2">
-        <v>9.8052769505345783</v>
+        <v>2.137101115036105</v>
       </c>
       <c r="G201" s="2">
-        <v>-0.44422008972081861</v>
+        <v>0.37016696058476473</v>
       </c>
       <c r="H201" s="2">
-        <v>-1.626183012561373</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-1.5905015295928231</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>208</v>
       </c>
@@ -6503,7 +6514,7 @@
         <v>-11.0586525236856</v>
       </c>
     </row>
-    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>209</v>
       </c>
@@ -6531,31 +6542,31 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>210</v>
+        <v>112</v>
       </c>
       <c r="B204" t="s">
         <v>235</v>
       </c>
       <c r="C204">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D204">
-        <v>697</v>
+        <v>161</v>
       </c>
       <c r="E204" s="2">
-        <v>26.414769697463729</v>
+        <v>4.5657843463384751</v>
       </c>
       <c r="F204" s="2">
-        <v>17.590745763539172</v>
+        <v>1.190512081949846</v>
       </c>
       <c r="G204" s="2">
-        <v>0.85967870253516132</v>
+        <v>0.17920735823326589</v>
       </c>
       <c r="H204" s="2">
-        <v>0.52585421434142776</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-1.921188741160909</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>211</v>
       </c>
@@ -6581,7 +6592,7 @@
         <v>-31.30568002527005</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>212</v>
       </c>
@@ -6607,7 +6618,7 @@
         <v>-10.372008321552221</v>
       </c>
     </row>
-    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>213</v>
       </c>
@@ -6633,7 +6644,7 @@
         <v>-13.905160873977859</v>
       </c>
     </row>
-    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>214</v>
       </c>
@@ -6659,7 +6670,7 @@
         <v>-33.150723849562532</v>
       </c>
     </row>
-    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>215</v>
       </c>
@@ -6685,7 +6696,7 @@
         <v>-25.55834742758163</v>
       </c>
     </row>
-    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>216</v>
       </c>
@@ -6711,7 +6722,7 @@
         <v>2.5581688654358281E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>217</v>
       </c>
@@ -6737,7 +6748,7 @@
         <v>-6.0334511928274352</v>
       </c>
     </row>
-    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>218</v>
       </c>
@@ -6763,7 +6774,7 @@
         <v>-6.1871884719444541</v>
       </c>
     </row>
-    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>219</v>
       </c>
@@ -6789,7 +6800,7 @@
         <v>-0.6973100075590779</v>
       </c>
     </row>
-    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>220</v>
       </c>
@@ -6815,7 +6826,7 @@
         <v>-2.2164714591850879E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>221</v>
       </c>
@@ -6843,31 +6854,31 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>222</v>
+        <v>129</v>
       </c>
       <c r="B216" t="s">
         <v>235</v>
       </c>
       <c r="C216">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="D216">
-        <v>991</v>
+        <v>156</v>
       </c>
       <c r="E216" s="2">
-        <v>0.51200329043375148</v>
+        <v>10.24904502767893</v>
       </c>
       <c r="F216" s="2">
-        <v>0.37918877089989661</v>
+        <v>3.9043811765291072</v>
       </c>
       <c r="G216" s="2">
-        <v>-0.50871948802159372</v>
+        <v>-0.18614511927025121</v>
       </c>
       <c r="H216" s="2">
-        <v>-0.50341315198099523</v>
-      </c>
-    </row>
-    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-8.5752698737579003</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>223</v>
       </c>
@@ -6893,7 +6904,7 @@
         <v>-10.669532448241039</v>
       </c>
     </row>
-    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>224</v>
       </c>
@@ -6921,83 +6932,83 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>225</v>
+        <v>36</v>
       </c>
       <c r="B219" t="s">
         <v>235</v>
       </c>
       <c r="C219">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D219">
-        <v>1527</v>
+        <v>154</v>
       </c>
       <c r="E219" s="2">
-        <v>51.81160325854551</v>
+        <v>7.4510885553505473</v>
       </c>
       <c r="F219" s="2">
-        <v>47.611500018495519</v>
+        <v>2.492613749837882</v>
       </c>
       <c r="G219" s="2">
-        <v>-2.3406745201743449</v>
+        <v>-0.22931039018344901</v>
       </c>
       <c r="H219" s="2">
-        <v>-2.4564784967956141</v>
+        <v>-7.1801972159013054</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>226</v>
+        <v>49</v>
       </c>
       <c r="B220" t="s">
         <v>235</v>
       </c>
       <c r="C220">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D220">
-        <v>1175</v>
+        <v>153</v>
       </c>
       <c r="E220" s="2">
-        <v>39.97566582969273</v>
+        <v>6.8862617191842768</v>
       </c>
       <c r="F220" s="2">
-        <v>28.941827434537348</v>
+        <v>2.7375989327663461</v>
       </c>
       <c r="G220" s="2">
-        <v>-0.63953932009518333</v>
+        <v>0.15723303348140469</v>
       </c>
       <c r="H220" s="2">
-        <v>-3.0399006229029282</v>
+        <v>-0.23697828441389679</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>227</v>
+        <v>24</v>
       </c>
       <c r="B221" t="s">
         <v>235</v>
       </c>
       <c r="C221">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="D221">
-        <v>2210</v>
+        <v>143</v>
       </c>
       <c r="E221" s="2">
-        <v>34.09935547955277</v>
+        <v>9.2480746628223827</v>
       </c>
       <c r="F221" s="2">
-        <v>25.097487683304269</v>
+        <v>3.2584483755467062</v>
       </c>
       <c r="G221" s="2">
-        <v>0.60528078994653289</v>
+        <v>0.2240466170549216</v>
       </c>
       <c r="H221" s="2">
-        <v>0.27772600976664891</v>
-      </c>
-    </row>
-    <row r="222" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>-4.5154638744299476</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>228</v>
       </c>
@@ -7023,7 +7034,7 @@
         <v>-44.946588015021852</v>
       </c>
     </row>
-    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>229</v>
       </c>
@@ -7049,7 +7060,7 @@
         <v>-5.453208210358591</v>
       </c>
     </row>
-    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>230</v>
       </c>
@@ -7075,7 +7086,7 @@
         <v>-20.61702161404391</v>
       </c>
     </row>
-    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>231</v>
       </c>
@@ -7103,11 +7114,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H225" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Running"/>
-      </filters>
-    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:H221">
+      <sortCondition descending="1" ref="D1:D225"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>